<commit_message>
Update buddingtonite analysis using XPP matrix correction method
</commit_message>
<xml_diff>
--- a/data/processed/buddingtonite_ANU/calczaf_files/calczaf_outputs.xlsx
+++ b/data/processed/buddingtonite_ANU/calczaf_files/calczaf_outputs.xlsx
@@ -479,31 +479,31 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>32.68</v>
+        <v>33.242</v>
       </c>
       <c r="C2">
-        <v>32.401</v>
+        <v>32.976</v>
       </c>
       <c r="D2">
-        <v>32.106</v>
+        <v>32.652</v>
       </c>
       <c r="E2">
-        <v>32.216</v>
+        <v>32.752</v>
       </c>
       <c r="F2">
-        <v>32.421</v>
+        <v>32.964</v>
       </c>
       <c r="G2">
-        <v>32.365</v>
+        <v>32.917</v>
       </c>
       <c r="H2">
-        <v>0.219</v>
+        <v>0.228</v>
       </c>
       <c r="I2">
-        <v>32.106</v>
+        <v>32.652</v>
       </c>
       <c r="J2">
-        <v>32.68</v>
+        <v>33.242</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -511,31 +511,31 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>9.992000000000001</v>
+        <v>10.148</v>
       </c>
       <c r="C3">
-        <v>10.102</v>
+        <v>10.266</v>
       </c>
       <c r="D3">
-        <v>10.087</v>
+        <v>10.242</v>
       </c>
       <c r="E3">
-        <v>10.099</v>
+        <v>10.25</v>
       </c>
       <c r="F3">
-        <v>9.978</v>
+        <v>10.13</v>
       </c>
       <c r="G3">
-        <v>10.052</v>
+        <v>10.207</v>
       </c>
       <c r="H3">
-        <v>0.061</v>
+        <v>0.063</v>
       </c>
       <c r="I3">
-        <v>9.978</v>
+        <v>10.13</v>
       </c>
       <c r="J3">
-        <v>10.102</v>
+        <v>10.266</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -546,19 +546,19 @@
         <v>0.025</v>
       </c>
       <c r="C4">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
       <c r="D4">
         <v>0.011</v>
       </c>
       <c r="E4">
-        <v>0.027</v>
+        <v>0.028</v>
       </c>
       <c r="F4">
         <v>0.027</v>
       </c>
       <c r="G4">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="H4">
         <v>0.008999999999999999</v>
@@ -567,7 +567,7 @@
         <v>0.011</v>
       </c>
       <c r="J4">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -575,31 +575,31 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.066</v>
+        <v>0.067</v>
       </c>
       <c r="C5">
-        <v>0.126</v>
+        <v>0.128</v>
       </c>
       <c r="D5">
-        <v>0.092</v>
+        <v>0.093</v>
       </c>
       <c r="E5">
-        <v>0.105</v>
+        <v>0.106</v>
       </c>
       <c r="F5">
-        <v>0.074</v>
+        <v>0.075</v>
       </c>
       <c r="G5">
-        <v>0.093</v>
+        <v>0.094</v>
       </c>
       <c r="H5">
         <v>0.024</v>
       </c>
       <c r="I5">
-        <v>0.066</v>
+        <v>0.067</v>
       </c>
       <c r="J5">
-        <v>0.126</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -607,31 +607,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1.171</v>
+        <v>1.259</v>
       </c>
       <c r="C6">
-        <v>1.223</v>
+        <v>1.316</v>
       </c>
       <c r="D6">
-        <v>1.129</v>
+        <v>1.214</v>
       </c>
       <c r="E6">
-        <v>1.094</v>
+        <v>1.176</v>
       </c>
       <c r="F6">
-        <v>1.112</v>
+        <v>1.196</v>
       </c>
       <c r="G6">
-        <v>1.146</v>
+        <v>1.232</v>
       </c>
       <c r="H6">
-        <v>0.052</v>
+        <v>0.056</v>
       </c>
       <c r="I6">
-        <v>1.094</v>
+        <v>1.176</v>
       </c>
       <c r="J6">
-        <v>1.223</v>
+        <v>1.316</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -639,31 +639,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>4.067</v>
+        <v>4.374</v>
       </c>
       <c r="C7">
-        <v>4.249</v>
+        <v>4.57</v>
       </c>
       <c r="D7">
-        <v>3.922</v>
+        <v>4.218</v>
       </c>
       <c r="E7">
-        <v>3.8</v>
+        <v>4.087</v>
       </c>
       <c r="F7">
-        <v>3.863</v>
+        <v>4.155</v>
       </c>
       <c r="G7">
-        <v>3.98</v>
+        <v>4.281</v>
       </c>
       <c r="H7">
-        <v>0.18</v>
+        <v>0.194</v>
       </c>
       <c r="I7">
-        <v>3.8</v>
+        <v>4.087</v>
       </c>
       <c r="J7">
-        <v>4.249</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -671,31 +671,31 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>48.472</v>
+        <v>49.428</v>
       </c>
       <c r="C8">
-        <v>48.38</v>
+        <v>49.364</v>
       </c>
       <c r="D8">
-        <v>47.827</v>
+        <v>48.757</v>
       </c>
       <c r="E8">
-        <v>47.901</v>
+        <v>48.811</v>
       </c>
       <c r="F8">
-        <v>48.052</v>
+        <v>48.973</v>
       </c>
       <c r="G8">
-        <v>48.127</v>
+        <v>49.067</v>
       </c>
       <c r="H8">
-        <v>0.287</v>
+        <v>0.312</v>
       </c>
       <c r="I8">
-        <v>47.827</v>
+        <v>48.757</v>
       </c>
       <c r="J8">
-        <v>48.472</v>
+        <v>49.428</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -703,31 +703,31 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>96.473</v>
+        <v>98.544</v>
       </c>
       <c r="C9">
-        <v>96.518</v>
+        <v>98.65600000000001</v>
       </c>
       <c r="D9">
-        <v>95.175</v>
+        <v>97.187</v>
       </c>
       <c r="E9">
-        <v>95.242</v>
+        <v>97.20999999999999</v>
       </c>
       <c r="F9">
-        <v>95.52800000000001</v>
+        <v>97.52</v>
       </c>
       <c r="G9">
-        <v>95.78700000000001</v>
+        <v>97.824</v>
       </c>
       <c r="H9">
-        <v>0.66</v>
+        <v>0.722</v>
       </c>
       <c r="I9">
-        <v>95.175</v>
+        <v>97.187</v>
       </c>
       <c r="J9">
-        <v>96.518</v>
+        <v>98.65600000000001</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -767,31 +767,31 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>69.913</v>
+        <v>71.117</v>
       </c>
       <c r="C12">
-        <v>69.316</v>
+        <v>70.54600000000001</v>
       </c>
       <c r="D12">
-        <v>68.68600000000001</v>
+        <v>69.854</v>
       </c>
       <c r="E12">
-        <v>68.92100000000001</v>
+        <v>70.068</v>
       </c>
       <c r="F12">
-        <v>69.35899999999999</v>
+        <v>70.52200000000001</v>
       </c>
       <c r="G12">
-        <v>69.239</v>
+        <v>70.42100000000001</v>
       </c>
       <c r="H12">
-        <v>0.469</v>
+        <v>0.489</v>
       </c>
       <c r="I12">
-        <v>68.68600000000001</v>
+        <v>69.854</v>
       </c>
       <c r="J12">
-        <v>69.913</v>
+        <v>71.117</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -799,31 +799,31 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>18.879</v>
+        <v>19.174</v>
       </c>
       <c r="C13">
-        <v>19.088</v>
+        <v>19.396</v>
       </c>
       <c r="D13">
-        <v>19.059</v>
+        <v>19.352</v>
       </c>
       <c r="E13">
-        <v>19.081</v>
+        <v>19.368</v>
       </c>
       <c r="F13">
-        <v>18.854</v>
+        <v>19.14</v>
       </c>
       <c r="G13">
-        <v>18.992</v>
+        <v>19.286</v>
       </c>
       <c r="H13">
-        <v>0.116</v>
+        <v>0.12</v>
       </c>
       <c r="I13">
-        <v>18.854</v>
+        <v>19.14</v>
       </c>
       <c r="J13">
-        <v>19.088</v>
+        <v>19.396</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -831,10 +831,10 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="C14">
-        <v>0.044</v>
+        <v>0.045</v>
       </c>
       <c r="D14">
         <v>0.013</v>
@@ -843,10 +843,10 @@
         <v>0.033</v>
       </c>
       <c r="F14">
-        <v>0.032</v>
+        <v>0.033</v>
       </c>
       <c r="G14">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="H14">
         <v>0.011</v>
@@ -855,7 +855,7 @@
         <v>0.013</v>
       </c>
       <c r="J14">
-        <v>0.044</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -866,28 +866,28 @@
         <v>0.09</v>
       </c>
       <c r="C15">
-        <v>0.17</v>
+        <v>0.172</v>
       </c>
       <c r="D15">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="E15">
-        <v>0.142</v>
+        <v>0.143</v>
       </c>
       <c r="F15">
-        <v>0.1</v>
+        <v>0.101</v>
       </c>
       <c r="G15">
-        <v>0.125</v>
+        <v>0.126</v>
       </c>
       <c r="H15">
-        <v>0.032</v>
+        <v>0.033</v>
       </c>
       <c r="I15">
         <v>0.09</v>
       </c>
       <c r="J15">
-        <v>0.17</v>
+        <v>0.172</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -895,31 +895,31 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>1.171</v>
+        <v>1.259</v>
       </c>
       <c r="C16">
-        <v>1.223</v>
+        <v>1.316</v>
       </c>
       <c r="D16">
-        <v>1.129</v>
+        <v>1.214</v>
       </c>
       <c r="E16">
-        <v>1.094</v>
+        <v>1.176</v>
       </c>
       <c r="F16">
-        <v>1.112</v>
+        <v>1.196</v>
       </c>
       <c r="G16">
-        <v>1.146</v>
+        <v>1.232</v>
       </c>
       <c r="H16">
-        <v>0.052</v>
+        <v>0.056</v>
       </c>
       <c r="I16">
-        <v>1.094</v>
+        <v>1.176</v>
       </c>
       <c r="J16">
-        <v>1.223</v>
+        <v>1.316</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -927,31 +927,31 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>6.39</v>
+        <v>6.873</v>
       </c>
       <c r="C17">
-        <v>6.676</v>
+        <v>7.18</v>
       </c>
       <c r="D17">
-        <v>6.162</v>
+        <v>6.627</v>
       </c>
       <c r="E17">
-        <v>5.971</v>
+        <v>6.421</v>
       </c>
       <c r="F17">
-        <v>6.07</v>
+        <v>6.528</v>
       </c>
       <c r="G17">
-        <v>6.254</v>
+        <v>6.726</v>
       </c>
       <c r="H17">
-        <v>0.282</v>
+        <v>0.304</v>
       </c>
       <c r="I17">
-        <v>5.971</v>
+        <v>6.421</v>
       </c>
       <c r="J17">
-        <v>6.676</v>
+        <v>7.18</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -959,31 +959,31 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>96.47199999999999</v>
+        <v>98.544</v>
       </c>
       <c r="C18">
-        <v>96.517</v>
+        <v>98.655</v>
       </c>
       <c r="D18">
-        <v>95.17400000000001</v>
+        <v>97.18600000000001</v>
       </c>
       <c r="E18">
-        <v>95.241</v>
+        <v>97.209</v>
       </c>
       <c r="F18">
-        <v>95.527</v>
+        <v>97.51900000000001</v>
       </c>
       <c r="G18">
-        <v>95.786</v>
+        <v>97.82299999999999</v>
       </c>
       <c r="H18">
-        <v>0.66</v>
+        <v>0.722</v>
       </c>
       <c r="I18">
-        <v>95.17400000000001</v>
+        <v>97.18600000000001</v>
       </c>
       <c r="J18">
-        <v>96.517</v>
+        <v>98.655</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1023,31 +1023,31 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>19.332</v>
+        <v>19.047</v>
       </c>
       <c r="C21">
-        <v>18.99</v>
+        <v>18.703</v>
       </c>
       <c r="D21">
-        <v>19.341</v>
+        <v>19.06</v>
       </c>
       <c r="E21">
-        <v>19.518</v>
+        <v>19.24</v>
       </c>
       <c r="F21">
-        <v>19.53</v>
+        <v>19.25</v>
       </c>
       <c r="G21">
-        <v>19.342</v>
+        <v>19.06</v>
       </c>
       <c r="H21">
-        <v>0.218</v>
+        <v>0.222</v>
       </c>
       <c r="I21">
-        <v>18.99</v>
+        <v>18.703</v>
       </c>
       <c r="J21">
-        <v>19.53</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1055,31 +1055,31 @@
         <v>6</v>
       </c>
       <c r="B22">
+        <v>6.052</v>
+      </c>
+      <c r="C22">
+        <v>6.06</v>
+      </c>
+      <c r="D22">
+        <v>6.223</v>
+      </c>
+      <c r="E22">
+        <v>6.268</v>
+      </c>
+      <c r="F22">
+        <v>6.158</v>
+      </c>
+      <c r="G22">
         <v>6.152</v>
-      </c>
-      <c r="C22">
-        <v>6.163</v>
-      </c>
-      <c r="D22">
-        <v>6.325</v>
-      </c>
-      <c r="E22">
-        <v>6.369</v>
-      </c>
-      <c r="F22">
-        <v>6.257</v>
-      </c>
-      <c r="G22">
-        <v>6.253</v>
       </c>
       <c r="H22">
         <v>0.096</v>
       </c>
       <c r="I22">
-        <v>6.152</v>
+        <v>6.052</v>
       </c>
       <c r="J22">
-        <v>6.369</v>
+        <v>6.268</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1087,7 +1087,7 @@
         <v>7</v>
       </c>
       <c r="B23">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="C23">
         <v>0.015</v>
@@ -1099,7 +1099,7 @@
         <v>0.012</v>
       </c>
       <c r="F23">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="G23">
         <v>0.011</v>
@@ -1119,31 +1119,31 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="C24">
-        <v>0.09</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D24">
-        <v>0.068</v>
+        <v>0.066</v>
       </c>
       <c r="E24">
-        <v>0.078</v>
+        <v>0.076</v>
       </c>
       <c r="F24">
-        <v>0.055</v>
+        <v>0.053</v>
       </c>
       <c r="G24">
-        <v>0.068</v>
+        <v>0.066</v>
       </c>
       <c r="H24">
         <v>0.017</v>
       </c>
       <c r="I24">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="J24">
-        <v>0.09</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1151,31 +1151,31 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>19.298</v>
+        <v>20.103</v>
       </c>
       <c r="C25">
-        <v>19.973</v>
+        <v>20.79</v>
       </c>
       <c r="D25">
-        <v>18.95</v>
+        <v>19.748</v>
       </c>
       <c r="E25">
-        <v>18.467</v>
+        <v>19.256</v>
       </c>
       <c r="F25">
-        <v>18.667</v>
+        <v>19.46</v>
       </c>
       <c r="G25">
-        <v>19.071</v>
+        <v>19.872</v>
       </c>
       <c r="H25">
-        <v>0.593</v>
+        <v>0.604</v>
       </c>
       <c r="I25">
-        <v>18.467</v>
+        <v>19.256</v>
       </c>
       <c r="J25">
-        <v>19.973</v>
+        <v>20.79</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1183,31 +1183,31 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>4.824</v>
+        <v>5.026</v>
       </c>
       <c r="C26">
-        <v>4.993</v>
+        <v>5.198</v>
       </c>
       <c r="D26">
-        <v>4.737</v>
+        <v>4.937</v>
       </c>
       <c r="E26">
-        <v>4.617</v>
+        <v>4.814</v>
       </c>
       <c r="F26">
-        <v>4.667</v>
+        <v>4.865</v>
       </c>
       <c r="G26">
-        <v>4.768</v>
+        <v>4.968</v>
       </c>
       <c r="H26">
-        <v>0.148</v>
+        <v>0.151</v>
       </c>
       <c r="I26">
-        <v>4.617</v>
+        <v>4.814</v>
       </c>
       <c r="J26">
-        <v>4.993</v>
+        <v>5.198</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1215,31 +1215,31 @@
         <v>11</v>
       </c>
       <c r="B27">
-        <v>50.334</v>
+        <v>49.714</v>
       </c>
       <c r="C27">
-        <v>49.774</v>
+        <v>49.146</v>
       </c>
       <c r="D27">
-        <v>50.574</v>
+        <v>49.96</v>
       </c>
       <c r="E27">
-        <v>50.941</v>
+        <v>50.333</v>
       </c>
       <c r="F27">
-        <v>50.813</v>
+        <v>50.202</v>
       </c>
       <c r="G27">
-        <v>50.487</v>
+        <v>49.871</v>
       </c>
       <c r="H27">
-        <v>0.461</v>
+        <v>0.469</v>
       </c>
       <c r="I27">
-        <v>49.774</v>
+        <v>49.146</v>
       </c>
       <c r="J27">
-        <v>50.941</v>
+        <v>50.333</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1327,31 +1327,31 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>32.693</v>
+        <v>33.263</v>
       </c>
       <c r="C2">
-        <v>32.411</v>
+        <v>32.993</v>
       </c>
       <c r="D2">
-        <v>32.119</v>
+        <v>32.673</v>
       </c>
       <c r="E2">
-        <v>32.227</v>
+        <v>32.776</v>
       </c>
       <c r="F2">
-        <v>32.43</v>
+        <v>32.982</v>
       </c>
       <c r="G2">
-        <v>32.376</v>
+        <v>32.938</v>
       </c>
       <c r="H2">
-        <v>0.22</v>
+        <v>0.228</v>
       </c>
       <c r="I2">
-        <v>32.119</v>
+        <v>32.673</v>
       </c>
       <c r="J2">
-        <v>32.693</v>
+        <v>33.263</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1359,31 +1359,31 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>9.997</v>
+        <v>10.156</v>
       </c>
       <c r="C3">
-        <v>10.106</v>
+        <v>10.272</v>
       </c>
       <c r="D3">
-        <v>10.092</v>
+        <v>10.25</v>
       </c>
       <c r="E3">
-        <v>10.103</v>
+        <v>10.259</v>
       </c>
       <c r="F3">
-        <v>9.981999999999999</v>
+        <v>10.136</v>
       </c>
       <c r="G3">
-        <v>10.056</v>
+        <v>10.215</v>
       </c>
       <c r="H3">
-        <v>0.061</v>
+        <v>0.064</v>
       </c>
       <c r="I3">
-        <v>9.981999999999999</v>
+        <v>10.136</v>
       </c>
       <c r="J3">
-        <v>10.106</v>
+        <v>10.272</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1394,19 +1394,19 @@
         <v>0.025</v>
       </c>
       <c r="C4">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
       <c r="D4">
         <v>0.011</v>
       </c>
       <c r="E4">
-        <v>0.027</v>
+        <v>0.028</v>
       </c>
       <c r="F4">
         <v>0.027</v>
       </c>
       <c r="G4">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="H4">
         <v>0.008999999999999999</v>
@@ -1415,7 +1415,7 @@
         <v>0.011</v>
       </c>
       <c r="J4">
-        <v>0.036</v>
+        <v>0.037</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1423,31 +1423,31 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.066</v>
+        <v>0.067</v>
       </c>
       <c r="C5">
-        <v>0.126</v>
+        <v>0.128</v>
       </c>
       <c r="D5">
-        <v>0.092</v>
+        <v>0.093</v>
       </c>
       <c r="E5">
-        <v>0.105</v>
+        <v>0.106</v>
       </c>
       <c r="F5">
-        <v>0.074</v>
+        <v>0.075</v>
       </c>
       <c r="G5">
-        <v>0.093</v>
+        <v>0.094</v>
       </c>
       <c r="H5">
         <v>0.024</v>
       </c>
       <c r="I5">
-        <v>0.066</v>
+        <v>0.067</v>
       </c>
       <c r="J5">
-        <v>0.126</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1455,31 +1455,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1.207</v>
+        <v>1.294</v>
       </c>
       <c r="C6">
-        <v>1.251</v>
+        <v>1.345</v>
       </c>
       <c r="D6">
-        <v>1.164</v>
+        <v>1.249</v>
       </c>
       <c r="E6">
-        <v>1.124</v>
+        <v>1.215</v>
       </c>
       <c r="F6">
-        <v>1.138</v>
+        <v>1.225</v>
       </c>
       <c r="G6">
-        <v>1.177</v>
+        <v>1.266</v>
       </c>
       <c r="H6">
-        <v>0.052</v>
+        <v>0.054</v>
       </c>
       <c r="I6">
-        <v>1.124</v>
+        <v>1.215</v>
       </c>
       <c r="J6">
-        <v>1.251</v>
+        <v>1.345</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1487,31 +1487,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>4.192</v>
+        <v>4.495</v>
       </c>
       <c r="C7">
-        <v>4.346</v>
+        <v>4.673</v>
       </c>
       <c r="D7">
-        <v>4.042</v>
+        <v>4.339</v>
       </c>
       <c r="E7">
-        <v>3.904</v>
+        <v>4.222</v>
       </c>
       <c r="F7">
-        <v>3.953</v>
+        <v>4.255</v>
       </c>
       <c r="G7">
-        <v>4.088</v>
+        <v>4.397</v>
       </c>
       <c r="H7">
-        <v>0.182</v>
+        <v>0.187</v>
       </c>
       <c r="I7">
-        <v>3.904</v>
+        <v>4.222</v>
       </c>
       <c r="J7">
-        <v>4.346</v>
+        <v>4.673</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1519,31 +1519,31 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>48.563</v>
+        <v>49.528</v>
       </c>
       <c r="C8">
-        <v>48.451</v>
+        <v>49.449</v>
       </c>
       <c r="D8">
-        <v>47.915</v>
+        <v>48.857</v>
       </c>
       <c r="E8">
-        <v>47.976</v>
+        <v>48.922</v>
       </c>
       <c r="F8">
-        <v>48.118</v>
+        <v>49.056</v>
       </c>
       <c r="G8">
-        <v>48.205</v>
+        <v>49.162</v>
       </c>
       <c r="H8">
-        <v>0.289</v>
+        <v>0.307</v>
       </c>
       <c r="I8">
-        <v>47.915</v>
+        <v>48.857</v>
       </c>
       <c r="J8">
-        <v>48.563</v>
+        <v>49.528</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1551,31 +1551,31 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>96.744</v>
+        <v>98.828</v>
       </c>
       <c r="C9">
-        <v>96.72799999999999</v>
+        <v>98.898</v>
       </c>
       <c r="D9">
-        <v>95.435</v>
+        <v>97.473</v>
       </c>
       <c r="E9">
-        <v>95.467</v>
+        <v>97.52800000000001</v>
       </c>
       <c r="F9">
-        <v>95.72199999999999</v>
+        <v>97.756</v>
       </c>
       <c r="G9">
-        <v>96.01900000000001</v>
+        <v>98.09699999999999</v>
       </c>
       <c r="H9">
-        <v>0.664</v>
+        <v>0.708</v>
       </c>
       <c r="I9">
-        <v>95.435</v>
+        <v>97.473</v>
       </c>
       <c r="J9">
-        <v>96.744</v>
+        <v>98.898</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1615,31 +1615,31 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>69.941</v>
+        <v>71.16200000000001</v>
       </c>
       <c r="C12">
-        <v>69.337</v>
+        <v>70.584</v>
       </c>
       <c r="D12">
-        <v>68.71299999999999</v>
+        <v>69.899</v>
       </c>
       <c r="E12">
-        <v>68.944</v>
+        <v>70.11799999999999</v>
       </c>
       <c r="F12">
-        <v>69.379</v>
+        <v>70.56</v>
       </c>
       <c r="G12">
-        <v>69.26300000000001</v>
+        <v>70.464</v>
       </c>
       <c r="H12">
-        <v>0.47</v>
+        <v>0.487</v>
       </c>
       <c r="I12">
-        <v>68.71299999999999</v>
+        <v>69.899</v>
       </c>
       <c r="J12">
-        <v>69.941</v>
+        <v>71.16200000000001</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1647,31 +1647,31 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>18.889</v>
+        <v>19.188</v>
       </c>
       <c r="C13">
-        <v>19.096</v>
+        <v>19.409</v>
       </c>
       <c r="D13">
-        <v>19.069</v>
+        <v>19.367</v>
       </c>
       <c r="E13">
-        <v>19.09</v>
+        <v>19.385</v>
       </c>
       <c r="F13">
-        <v>18.861</v>
+        <v>19.152</v>
       </c>
       <c r="G13">
-        <v>19.001</v>
+        <v>19.3</v>
       </c>
       <c r="H13">
-        <v>0.116</v>
+        <v>0.12</v>
       </c>
       <c r="I13">
-        <v>18.861</v>
+        <v>19.152</v>
       </c>
       <c r="J13">
-        <v>19.096</v>
+        <v>19.409</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1679,10 +1679,10 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="C14">
-        <v>0.044</v>
+        <v>0.045</v>
       </c>
       <c r="D14">
         <v>0.013</v>
@@ -1691,10 +1691,10 @@
         <v>0.033</v>
       </c>
       <c r="F14">
-        <v>0.032</v>
+        <v>0.033</v>
       </c>
       <c r="G14">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="H14">
         <v>0.011</v>
@@ -1703,7 +1703,7 @@
         <v>0.013</v>
       </c>
       <c r="J14">
-        <v>0.044</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1714,28 +1714,28 @@
         <v>0.09</v>
       </c>
       <c r="C15">
-        <v>0.17</v>
+        <v>0.172</v>
       </c>
       <c r="D15">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="E15">
-        <v>0.142</v>
+        <v>0.143</v>
       </c>
       <c r="F15">
-        <v>0.1</v>
+        <v>0.101</v>
       </c>
       <c r="G15">
-        <v>0.125</v>
+        <v>0.126</v>
       </c>
       <c r="H15">
-        <v>0.032</v>
+        <v>0.033</v>
       </c>
       <c r="I15">
         <v>0.09</v>
       </c>
       <c r="J15">
-        <v>0.17</v>
+        <v>0.172</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1743,31 +1743,31 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>1.207</v>
+        <v>1.294</v>
       </c>
       <c r="C16">
-        <v>1.251</v>
+        <v>1.345</v>
       </c>
       <c r="D16">
-        <v>1.164</v>
+        <v>1.249</v>
       </c>
       <c r="E16">
-        <v>1.124</v>
+        <v>1.215</v>
       </c>
       <c r="F16">
-        <v>1.138</v>
+        <v>1.225</v>
       </c>
       <c r="G16">
-        <v>1.177</v>
+        <v>1.266</v>
       </c>
       <c r="H16">
-        <v>0.052</v>
+        <v>0.054</v>
       </c>
       <c r="I16">
-        <v>1.124</v>
+        <v>1.215</v>
       </c>
       <c r="J16">
-        <v>1.251</v>
+        <v>1.345</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1775,31 +1775,31 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>6.587</v>
+        <v>7.062</v>
       </c>
       <c r="C17">
-        <v>6.829</v>
+        <v>7.342</v>
       </c>
       <c r="D17">
-        <v>6.351</v>
+        <v>6.818</v>
       </c>
       <c r="E17">
-        <v>6.134</v>
+        <v>6.633</v>
       </c>
       <c r="F17">
-        <v>6.211</v>
+        <v>6.686</v>
       </c>
       <c r="G17">
-        <v>6.422</v>
+        <v>6.908</v>
       </c>
       <c r="H17">
-        <v>0.285</v>
+        <v>0.294</v>
       </c>
       <c r="I17">
-        <v>6.134</v>
+        <v>6.633</v>
       </c>
       <c r="J17">
-        <v>6.829</v>
+        <v>7.342</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1807,31 +1807,31 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>96.74299999999999</v>
+        <v>98.827</v>
       </c>
       <c r="C18">
-        <v>96.727</v>
+        <v>98.89700000000001</v>
       </c>
       <c r="D18">
-        <v>95.434</v>
+        <v>97.47199999999999</v>
       </c>
       <c r="E18">
-        <v>95.46599999999999</v>
+        <v>97.527</v>
       </c>
       <c r="F18">
-        <v>95.721</v>
+        <v>97.756</v>
       </c>
       <c r="G18">
-        <v>96.018</v>
+        <v>98.096</v>
       </c>
       <c r="H18">
-        <v>0.664</v>
+        <v>0.708</v>
       </c>
       <c r="I18">
-        <v>95.434</v>
+        <v>97.47199999999999</v>
       </c>
       <c r="J18">
-        <v>96.74299999999999</v>
+        <v>98.89700000000001</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1871,31 +1871,31 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>19.177</v>
+        <v>18.906</v>
       </c>
       <c r="C21">
-        <v>18.872</v>
+        <v>18.585</v>
       </c>
       <c r="D21">
-        <v>19.189</v>
+        <v>18.916</v>
       </c>
       <c r="E21">
-        <v>19.384</v>
+        <v>19.077</v>
       </c>
       <c r="F21">
-        <v>19.416</v>
+        <v>19.129</v>
       </c>
       <c r="G21">
-        <v>19.208</v>
+        <v>18.923</v>
       </c>
       <c r="H21">
-        <v>0.217</v>
+        <v>0.212</v>
       </c>
       <c r="I21">
-        <v>18.872</v>
+        <v>18.585</v>
       </c>
       <c r="J21">
-        <v>19.416</v>
+        <v>19.129</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1903,31 +1903,31 @@
         <v>6</v>
       </c>
       <c r="B22">
-        <v>6.104</v>
+        <v>6.008</v>
       </c>
       <c r="C22">
-        <v>6.126</v>
+        <v>6.023</v>
       </c>
       <c r="D22">
-        <v>6.276</v>
+        <v>6.177</v>
       </c>
       <c r="E22">
-        <v>6.326</v>
+        <v>6.216</v>
       </c>
       <c r="F22">
-        <v>6.221</v>
+        <v>6.119</v>
       </c>
       <c r="G22">
-        <v>6.211</v>
+        <v>6.109</v>
       </c>
       <c r="H22">
-        <v>0.095</v>
+        <v>0.092</v>
       </c>
       <c r="I22">
-        <v>6.104</v>
+        <v>6.008</v>
       </c>
       <c r="J22">
-        <v>6.326</v>
+        <v>6.216</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1947,7 +1947,7 @@
         <v>0.012</v>
       </c>
       <c r="F23">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="G23">
         <v>0.011</v>
@@ -1967,31 +1967,31 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="C24">
-        <v>0.09</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D24">
-        <v>0.067</v>
+        <v>0.066</v>
       </c>
       <c r="E24">
-        <v>0.077</v>
+        <v>0.075</v>
       </c>
       <c r="F24">
-        <v>0.054</v>
+        <v>0.053</v>
       </c>
       <c r="G24">
-        <v>0.067</v>
+        <v>0.066</v>
       </c>
       <c r="H24">
         <v>0.017</v>
       </c>
       <c r="I24">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="J24">
-        <v>0.09</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1999,31 +1999,31 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>19.725</v>
+        <v>20.492</v>
       </c>
       <c r="C25">
-        <v>20.299</v>
+        <v>21.114</v>
       </c>
       <c r="D25">
-        <v>19.37</v>
+        <v>20.149</v>
       </c>
       <c r="E25">
-        <v>18.835</v>
+        <v>19.708</v>
       </c>
       <c r="F25">
-        <v>18.982</v>
+        <v>19.795</v>
       </c>
       <c r="G25">
-        <v>19.442</v>
+        <v>20.252</v>
       </c>
       <c r="H25">
-        <v>0.591</v>
+        <v>0.574</v>
       </c>
       <c r="I25">
-        <v>18.835</v>
+        <v>19.708</v>
       </c>
       <c r="J25">
-        <v>20.299</v>
+        <v>21.114</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2031,31 +2031,31 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>4.931</v>
+        <v>5.123</v>
       </c>
       <c r="C26">
-        <v>5.075</v>
+        <v>5.279</v>
       </c>
       <c r="D26">
-        <v>4.843</v>
+        <v>5.037</v>
       </c>
       <c r="E26">
-        <v>4.709</v>
+        <v>4.927</v>
       </c>
       <c r="F26">
-        <v>4.746</v>
+        <v>4.949</v>
       </c>
       <c r="G26">
-        <v>4.861</v>
+        <v>5.063</v>
       </c>
       <c r="H26">
-        <v>0.148</v>
+        <v>0.143</v>
       </c>
       <c r="I26">
-        <v>4.709</v>
+        <v>4.927</v>
       </c>
       <c r="J26">
-        <v>5.075</v>
+        <v>5.279</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2063,31 +2063,31 @@
         <v>11</v>
       </c>
       <c r="B27">
-        <v>50.005</v>
+        <v>49.414</v>
       </c>
       <c r="C27">
-        <v>49.523</v>
+        <v>48.896</v>
       </c>
       <c r="D27">
-        <v>50.25</v>
+        <v>49.651</v>
       </c>
       <c r="E27">
-        <v>50.657</v>
+        <v>49.985</v>
       </c>
       <c r="F27">
-        <v>50.57</v>
+        <v>49.944</v>
       </c>
       <c r="G27">
-        <v>50.201</v>
+        <v>49.578</v>
       </c>
       <c r="H27">
-        <v>0.459</v>
+        <v>0.446</v>
       </c>
       <c r="I27">
-        <v>49.523</v>
+        <v>48.896</v>
       </c>
       <c r="J27">
-        <v>50.657</v>
+        <v>49.985</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2175,31 +2175,31 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>32.781</v>
+        <v>33.434</v>
       </c>
       <c r="C2">
-        <v>32.501</v>
+        <v>33.153</v>
       </c>
       <c r="D2">
-        <v>32.198</v>
+        <v>32.827</v>
       </c>
       <c r="E2">
-        <v>32.31</v>
+        <v>32.927</v>
       </c>
       <c r="F2">
-        <v>32.508</v>
+        <v>33.146</v>
       </c>
       <c r="G2">
-        <v>32.459</v>
+        <v>33.097</v>
       </c>
       <c r="H2">
-        <v>0.223</v>
+        <v>0.235</v>
       </c>
       <c r="I2">
-        <v>32.198</v>
+        <v>32.827</v>
       </c>
       <c r="J2">
-        <v>32.781</v>
+        <v>33.434</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2207,31 +2207,31 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>10.03</v>
+        <v>10.211</v>
       </c>
       <c r="C3">
-        <v>10.15</v>
+        <v>10.334</v>
       </c>
       <c r="D3">
-        <v>10.132</v>
+        <v>10.304</v>
       </c>
       <c r="E3">
-        <v>10.137</v>
+        <v>10.316</v>
       </c>
       <c r="F3">
-        <v>10.02</v>
+        <v>10.193</v>
       </c>
       <c r="G3">
-        <v>10.094</v>
+        <v>10.272</v>
       </c>
       <c r="H3">
-        <v>0.063</v>
+        <v>0.065</v>
       </c>
       <c r="I3">
-        <v>10.02</v>
+        <v>10.193</v>
       </c>
       <c r="J3">
-        <v>10.15</v>
+        <v>10.334</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2239,13 +2239,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.026</v>
+        <v>0.025</v>
       </c>
       <c r="C4">
-        <v>0.036</v>
+        <v>0.038</v>
       </c>
       <c r="D4">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="E4">
         <v>0.028</v>
@@ -2257,13 +2257,13 @@
         <v>0.026</v>
       </c>
       <c r="H4">
-        <v>0.008999999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="I4">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="J4">
-        <v>0.036</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2271,31 +2271,31 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.065</v>
+        <v>0.066</v>
       </c>
       <c r="C5">
-        <v>0.127</v>
+        <v>0.126</v>
       </c>
       <c r="D5">
-        <v>0.095</v>
+        <v>0.092</v>
       </c>
       <c r="E5">
-        <v>0.104</v>
+        <v>0.108</v>
       </c>
       <c r="F5">
-        <v>0.077</v>
+        <v>0.074</v>
       </c>
       <c r="G5">
         <v>0.093</v>
       </c>
       <c r="H5">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="I5">
-        <v>0.065</v>
+        <v>0.066</v>
       </c>
       <c r="J5">
-        <v>0.127</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2303,31 +2303,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1.461</v>
+        <v>1.567</v>
       </c>
       <c r="C6">
-        <v>1.514</v>
+        <v>1.629</v>
       </c>
       <c r="D6">
-        <v>1.409</v>
+        <v>1.513</v>
       </c>
       <c r="E6">
-        <v>1.361</v>
+        <v>1.472</v>
       </c>
       <c r="F6">
-        <v>1.378</v>
+        <v>1.484</v>
       </c>
       <c r="G6">
-        <v>1.425</v>
+        <v>1.533</v>
       </c>
       <c r="H6">
-        <v>0.063</v>
+        <v>0.065</v>
       </c>
       <c r="I6">
-        <v>1.361</v>
+        <v>1.472</v>
       </c>
       <c r="J6">
-        <v>1.514</v>
+        <v>1.629</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2335,31 +2335,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>5.076</v>
+        <v>5.445</v>
       </c>
       <c r="C7">
-        <v>5.261</v>
+        <v>5.659</v>
       </c>
       <c r="D7">
-        <v>4.895</v>
+        <v>5.257</v>
       </c>
       <c r="E7">
-        <v>4.729</v>
+        <v>5.115</v>
       </c>
       <c r="F7">
-        <v>4.787</v>
+        <v>5.156</v>
       </c>
       <c r="G7">
-        <v>4.949</v>
+        <v>5.327</v>
       </c>
       <c r="H7">
-        <v>0.218</v>
+        <v>0.226</v>
       </c>
       <c r="I7">
-        <v>4.729</v>
+        <v>5.115</v>
       </c>
       <c r="J7">
-        <v>5.261</v>
+        <v>5.659</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2367,31 +2367,31 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>49.197</v>
+        <v>50.314</v>
       </c>
       <c r="C8">
-        <v>49.115</v>
+        <v>50.25</v>
       </c>
       <c r="D8">
-        <v>48.528</v>
+        <v>49.604</v>
       </c>
       <c r="E8">
-        <v>48.572</v>
+        <v>49.656</v>
       </c>
       <c r="F8">
-        <v>48.717</v>
+        <v>49.807</v>
       </c>
       <c r="G8">
-        <v>48.826</v>
+        <v>49.926</v>
       </c>
       <c r="H8">
-        <v>0.311</v>
+        <v>0.334</v>
       </c>
       <c r="I8">
-        <v>48.528</v>
+        <v>49.604</v>
       </c>
       <c r="J8">
-        <v>49.197</v>
+        <v>50.314</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2399,31 +2399,31 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>98.63500000000001</v>
+        <v>101.063</v>
       </c>
       <c r="C9">
-        <v>98.70399999999999</v>
+        <v>101.19</v>
       </c>
       <c r="D9">
-        <v>97.26900000000001</v>
+        <v>99.608</v>
       </c>
       <c r="E9">
-        <v>97.241</v>
+        <v>99.624</v>
       </c>
       <c r="F9">
-        <v>97.51300000000001</v>
+        <v>99.886</v>
       </c>
       <c r="G9">
-        <v>97.873</v>
+        <v>100.274</v>
       </c>
       <c r="H9">
-        <v>0.736</v>
+        <v>0.787</v>
       </c>
       <c r="I9">
-        <v>97.241</v>
+        <v>99.608</v>
       </c>
       <c r="J9">
-        <v>98.70399999999999</v>
+        <v>101.19</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2463,31 +2463,31 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>70.129</v>
+        <v>71.527</v>
       </c>
       <c r="C12">
-        <v>69.53</v>
+        <v>70.926</v>
       </c>
       <c r="D12">
-        <v>68.88200000000001</v>
+        <v>70.22799999999999</v>
       </c>
       <c r="E12">
-        <v>69.122</v>
+        <v>70.441</v>
       </c>
       <c r="F12">
-        <v>69.545</v>
+        <v>70.90900000000001</v>
       </c>
       <c r="G12">
-        <v>69.44199999999999</v>
+        <v>70.806</v>
       </c>
       <c r="H12">
-        <v>0.476</v>
+        <v>0.503</v>
       </c>
       <c r="I12">
-        <v>68.88200000000001</v>
+        <v>70.22799999999999</v>
       </c>
       <c r="J12">
-        <v>70.129</v>
+        <v>71.527</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2495,31 +2495,31 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>18.952</v>
+        <v>19.294</v>
       </c>
       <c r="C13">
-        <v>19.179</v>
+        <v>19.526</v>
       </c>
       <c r="D13">
-        <v>19.144</v>
+        <v>19.469</v>
       </c>
       <c r="E13">
-        <v>19.154</v>
+        <v>19.493</v>
       </c>
       <c r="F13">
-        <v>18.932</v>
+        <v>19.26</v>
       </c>
       <c r="G13">
-        <v>19.072</v>
+        <v>19.408</v>
       </c>
       <c r="H13">
-        <v>0.12</v>
+        <v>0.122</v>
       </c>
       <c r="I13">
-        <v>18.932</v>
+        <v>19.26</v>
       </c>
       <c r="J13">
-        <v>19.179</v>
+        <v>19.526</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2527,13 +2527,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="C14">
-        <v>0.044</v>
+        <v>0.046</v>
       </c>
       <c r="D14">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
       <c r="E14">
         <v>0.034</v>
@@ -2545,13 +2545,13 @@
         <v>0.031</v>
       </c>
       <c r="H14">
-        <v>0.011</v>
+        <v>0.012</v>
       </c>
       <c r="I14">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
       <c r="J14">
-        <v>0.044</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2559,19 +2559,19 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0.08699999999999999</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="C15">
         <v>0.171</v>
       </c>
       <c r="D15">
-        <v>0.129</v>
+        <v>0.124</v>
       </c>
       <c r="E15">
-        <v>0.14</v>
+        <v>0.146</v>
       </c>
       <c r="F15">
-        <v>0.103</v>
+        <v>0.099</v>
       </c>
       <c r="G15">
         <v>0.126</v>
@@ -2580,7 +2580,7 @@
         <v>0.033</v>
       </c>
       <c r="I15">
-        <v>0.08699999999999999</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="J15">
         <v>0.171</v>
@@ -2591,31 +2591,31 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>1.461</v>
+        <v>1.567</v>
       </c>
       <c r="C16">
-        <v>1.514</v>
+        <v>1.629</v>
       </c>
       <c r="D16">
-        <v>1.409</v>
+        <v>1.513</v>
       </c>
       <c r="E16">
-        <v>1.361</v>
+        <v>1.472</v>
       </c>
       <c r="F16">
-        <v>1.378</v>
+        <v>1.484</v>
       </c>
       <c r="G16">
-        <v>1.425</v>
+        <v>1.533</v>
       </c>
       <c r="H16">
-        <v>0.063</v>
+        <v>0.065</v>
       </c>
       <c r="I16">
-        <v>1.361</v>
+        <v>1.472</v>
       </c>
       <c r="J16">
-        <v>1.514</v>
+        <v>1.629</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2623,31 +2623,31 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>7.975</v>
+        <v>8.555</v>
       </c>
       <c r="C17">
-        <v>8.265000000000001</v>
+        <v>8.891999999999999</v>
       </c>
       <c r="D17">
-        <v>7.69</v>
+        <v>8.259</v>
       </c>
       <c r="E17">
-        <v>7.429</v>
+        <v>8.037000000000001</v>
       </c>
       <c r="F17">
-        <v>7.522</v>
+        <v>8.101000000000001</v>
       </c>
       <c r="G17">
-        <v>7.776</v>
+        <v>8.369</v>
       </c>
       <c r="H17">
-        <v>0.343</v>
+        <v>0.354</v>
       </c>
       <c r="I17">
-        <v>7.429</v>
+        <v>8.037000000000001</v>
       </c>
       <c r="J17">
-        <v>8.265000000000001</v>
+        <v>8.891999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2655,31 +2655,31 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>98.63500000000001</v>
+        <v>101.062</v>
       </c>
       <c r="C18">
-        <v>98.703</v>
+        <v>101.189</v>
       </c>
       <c r="D18">
-        <v>97.268</v>
+        <v>99.608</v>
       </c>
       <c r="E18">
-        <v>97.23999999999999</v>
+        <v>99.623</v>
       </c>
       <c r="F18">
-        <v>97.512</v>
+        <v>99.886</v>
       </c>
       <c r="G18">
-        <v>97.872</v>
+        <v>100.273</v>
       </c>
       <c r="H18">
-        <v>0.736</v>
+        <v>0.787</v>
       </c>
       <c r="I18">
-        <v>97.23999999999999</v>
+        <v>99.608</v>
       </c>
       <c r="J18">
-        <v>98.703</v>
+        <v>101.189</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2719,31 +2719,31 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>18.155</v>
+        <v>17.872</v>
       </c>
       <c r="C21">
-        <v>17.838</v>
+        <v>17.538</v>
       </c>
       <c r="D21">
-        <v>18.178</v>
+        <v>17.894</v>
       </c>
       <c r="E21">
-        <v>18.391</v>
+        <v>18.065</v>
       </c>
       <c r="F21">
-        <v>18.411</v>
+        <v>18.114</v>
       </c>
       <c r="G21">
-        <v>18.194</v>
+        <v>17.897</v>
       </c>
       <c r="H21">
-        <v>0.232</v>
+        <v>0.226</v>
       </c>
       <c r="I21">
-        <v>17.838</v>
+        <v>17.538</v>
       </c>
       <c r="J21">
-        <v>18.411</v>
+        <v>18.114</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2751,31 +2751,31 @@
         <v>6</v>
       </c>
       <c r="B22">
+        <v>5.682</v>
+      </c>
+      <c r="C22">
+        <v>5.69</v>
+      </c>
+      <c r="D22">
+        <v>5.847</v>
+      </c>
+      <c r="E22">
+        <v>5.892</v>
+      </c>
+      <c r="F22">
+        <v>5.798</v>
+      </c>
+      <c r="G22">
         <v>5.782</v>
       </c>
-      <c r="C22">
-        <v>5.799</v>
-      </c>
-      <c r="D22">
-        <v>5.954</v>
-      </c>
-      <c r="E22">
-        <v>6.006</v>
-      </c>
-      <c r="F22">
-        <v>5.907</v>
-      </c>
-      <c r="G22">
-        <v>5.89</v>
-      </c>
       <c r="H22">
-        <v>0.097</v>
+        <v>0.093</v>
       </c>
       <c r="I22">
-        <v>5.782</v>
+        <v>5.682</v>
       </c>
       <c r="J22">
-        <v>6.006</v>
+        <v>5.892</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2789,13 +2789,13 @@
         <v>0.014</v>
       </c>
       <c r="D23">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="E23">
         <v>0.011</v>
       </c>
       <c r="F23">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="G23">
         <v>0.01</v>
@@ -2804,7 +2804,7 @@
         <v>0.004</v>
       </c>
       <c r="I23">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="J23">
         <v>0.014</v>
@@ -2815,31 +2815,31 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="C24">
-        <v>0.08500000000000001</v>
+        <v>0.082</v>
       </c>
       <c r="D24">
-        <v>0.066</v>
+        <v>0.061</v>
       </c>
       <c r="E24">
         <v>0.07199999999999999</v>
       </c>
       <c r="F24">
-        <v>0.053</v>
+        <v>0.049</v>
       </c>
       <c r="G24">
-        <v>0.064</v>
+        <v>0.062</v>
       </c>
       <c r="H24">
         <v>0.016</v>
       </c>
       <c r="I24">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="J24">
-        <v>0.08500000000000001</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2847,31 +2847,31 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>22.546</v>
+        <v>23.345</v>
       </c>
       <c r="C25">
-        <v>23.157</v>
+        <v>24.012</v>
       </c>
       <c r="D25">
-        <v>22.164</v>
+        <v>22.984</v>
       </c>
       <c r="E25">
-        <v>21.589</v>
+        <v>22.51</v>
       </c>
       <c r="F25">
-        <v>21.747</v>
+        <v>22.599</v>
       </c>
       <c r="G25">
-        <v>22.241</v>
+        <v>23.09</v>
       </c>
       <c r="H25">
-        <v>0.634</v>
+        <v>0.613</v>
       </c>
       <c r="I25">
-        <v>21.589</v>
+        <v>22.51</v>
       </c>
       <c r="J25">
-        <v>23.157</v>
+        <v>24.012</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2879,31 +2879,31 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>5.636</v>
+        <v>5.836</v>
       </c>
       <c r="C26">
-        <v>5.789</v>
+        <v>6.003</v>
       </c>
       <c r="D26">
-        <v>5.541</v>
+        <v>5.746</v>
       </c>
       <c r="E26">
-        <v>5.397</v>
+        <v>5.627</v>
       </c>
       <c r="F26">
-        <v>5.437</v>
+        <v>5.65</v>
       </c>
       <c r="G26">
-        <v>5.56</v>
+        <v>5.772</v>
       </c>
       <c r="H26">
-        <v>0.159</v>
+        <v>0.153</v>
       </c>
       <c r="I26">
-        <v>5.397</v>
+        <v>5.627</v>
       </c>
       <c r="J26">
-        <v>5.789</v>
+        <v>6.003</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2911,31 +2911,31 @@
         <v>11</v>
       </c>
       <c r="B27">
-        <v>47.827</v>
+        <v>47.212</v>
       </c>
       <c r="C27">
-        <v>47.318</v>
+        <v>46.661</v>
       </c>
       <c r="D27">
-        <v>48.092</v>
+        <v>47.464</v>
       </c>
       <c r="E27">
-        <v>48.533</v>
+        <v>47.823</v>
       </c>
       <c r="F27">
-        <v>48.434</v>
+        <v>47.78</v>
       </c>
       <c r="G27">
-        <v>48.041</v>
+        <v>47.388</v>
       </c>
       <c r="H27">
-        <v>0.492</v>
+        <v>0.476</v>
       </c>
       <c r="I27">
-        <v>47.318</v>
+        <v>46.661</v>
       </c>
       <c r="J27">
-        <v>48.533</v>
+        <v>47.823</v>
       </c>
     </row>
     <row r="28" spans="1:10">

</xml_diff>